<commit_message>
Cambios finales de la version 4.1.12
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteAnulacion.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteAnulacion.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Empeños\Comprobantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtjarquinm\Documents\GitHub-Donovan\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A26433-CF9F-49AA-B5D9-1444BB22A155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3492" windowWidth="28800" windowHeight="15456"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">CASA DE EMPEÑOS </t>
   </si>
@@ -90,15 +91,18 @@
   </si>
   <si>
     <t>Comprobante de Anulación</t>
+  </si>
+  <si>
+    <t>N° Anulacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -254,9 +258,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -295,8 +299,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,10 +339,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -335,32 +367,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -642,134 +649,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:B28"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.109375" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="51.109375" customWidth="1"/>
+    <col min="1" max="1" width="50.08984375" customWidth="1"/>
+    <col min="2" max="2" width="42.6328125" customWidth="1"/>
+    <col min="4" max="4" width="51.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.4" x14ac:dyDescent="0.7">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-    </row>
-    <row r="2" spans="1:4" ht="64.95" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A2" s="29" t="s">
+    <row r="1" spans="1:4" ht="44.5" x14ac:dyDescent="0.85">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" ht="65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A3" s="29" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-    </row>
-    <row r="4" spans="1:4" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:4" ht="122" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-    </row>
-    <row r="5" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A5" s="29" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+    </row>
+    <row r="5" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="6" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A6" s="29" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-    </row>
-    <row r="7" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A7" s="29" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-    </row>
-    <row r="8" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A8" s="6"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A8" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="52.2" customHeight="1" x14ac:dyDescent="0.95">
+    <row r="9" spans="1:4" ht="52.25" customHeight="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-    </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A16" s="15" t="s">
         <v>15</v>
       </c>
@@ -777,15 +786,15 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="1.1000000000000001">
+    <row r="17" spans="1:4" ht="70" x14ac:dyDescent="1.35">
       <c r="A17" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -793,160 +802,146 @@
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-    </row>
-    <row r="21" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A22" s="19" t="s">
+    <row r="19" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A22" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="33">
+      <c r="B22" s="20"/>
+      <c r="C22" s="19">
         <v>0</v>
       </c>
-      <c r="D22" s="33"/>
-    </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A23" s="19" t="s">
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A23" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="38">
+      <c r="B23" s="20"/>
+      <c r="C23" s="25">
         <v>0</v>
       </c>
-      <c r="D23" s="38"/>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A24" s="19" t="s">
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A24" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20">
+      <c r="B24" s="20"/>
+      <c r="C24" s="30">
         <v>43501</v>
       </c>
-      <c r="D24" s="20"/>
-    </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="D24" s="30"/>
+    </row>
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A26" s="32" t="s">
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A26" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A28" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B28" s="20"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+    </row>
+    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A31" s="22" t="s">
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+    </row>
+    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A31" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-    </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+    </row>
+    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-    </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A34" s="22" t="s">
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A34" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-    </row>
-    <row r="35" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24" t="s">
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+    </row>
+    <row r="35" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-    </row>
-    <row r="36" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-    </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A37" s="18" t="s">
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+    </row>
+    <row r="36" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A37" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A19:D21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A24:B24"/>
@@ -963,6 +958,20 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A19:D21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="21" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>